<commit_message>
completed 10 test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data.xlsx
+++ b/src/test/resources/test_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\IdeaProjects\winterweekendselenium\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahya\IdeaProjects\AssignmentTwo\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FAB92B-8EC5-40F3-8A4C-F1EDDEB92F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B361D7BF-8CF8-4603-8AFC-4E5C60786F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{737F456A-BA07-46AB-AAA2-7DD47C4B7DA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{737F456A-BA07-46AB-AAA2-7DD47C4B7DA6}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginValidEmailInvalidPass" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>User</t>
   </si>
@@ -44,73 +44,91 @@
     <t>Password</t>
   </si>
   <si>
-    <t>abdi@netflix.com</t>
-  </si>
-  <si>
-    <t>sami@gmail.com</t>
-  </si>
-  <si>
-    <t>kjahsdfkjklj</t>
-  </si>
-  <si>
     <t>*&amp;(^(*&amp;%%^&amp;$</t>
   </si>
   <si>
-    <t>kjhasf78876</t>
-  </si>
-  <si>
-    <t>asdkjh78322##$$</t>
-  </si>
-  <si>
-    <t>tadefi_01@yahoo.fr</t>
-  </si>
-  <si>
-    <t>abbagaroj@gmail.com</t>
-  </si>
-  <si>
-    <t>kyliejenner@me.com</t>
-  </si>
-  <si>
-    <t>aghilesham20@yahoo.com</t>
-  </si>
-  <si>
-    <t>asdf4334</t>
-  </si>
-  <si>
-    <t>adsfgih3487</t>
-  </si>
-  <si>
-    <t>asdf3q4t34yt</t>
-  </si>
-  <si>
-    <t>adsg4355</t>
-  </si>
-  <si>
-    <t>bvncvbm54*&amp;%^#</t>
-  </si>
-  <si>
-    <t>klasjd</t>
-  </si>
-  <si>
-    <t>asd;lk2@</t>
-  </si>
-  <si>
-    <t>abdi@netflix</t>
-  </si>
-  <si>
-    <t>abbagaroj@gmail.co</t>
-  </si>
-  <si>
-    <t>sami@gmailcom</t>
-  </si>
-  <si>
-    <t>kyliejennerme.com</t>
-  </si>
-  <si>
-    <t>tadefi_01@yahoo.f</t>
-  </si>
-  <si>
-    <t>aghilesham20@yahoo.cm</t>
+    <t>yahyaq91@gmail.com</t>
+  </si>
+  <si>
+    <t>yahyaq91@yahoo.com</t>
+  </si>
+  <si>
+    <t>yahyaq91@live.com</t>
+  </si>
+  <si>
+    <t>nufc@hotmail.com</t>
+  </si>
+  <si>
+    <t>realmadrid@live.com</t>
+  </si>
+  <si>
+    <t>ronaldo9@icloud.com</t>
+  </si>
+  <si>
+    <t>cronaldo7@me.com</t>
+  </si>
+  <si>
+    <t>haaland@gmail.com</t>
+  </si>
+  <si>
+    <t>fddfasdfd</t>
+  </si>
+  <si>
+    <t>saddf7463</t>
+  </si>
+  <si>
+    <t>dsda%%^</t>
+  </si>
+  <si>
+    <t>dsas*&amp;^#432</t>
+  </si>
+  <si>
+    <t>%$#^ffaw</t>
+  </si>
+  <si>
+    <t>dfadfdag</t>
+  </si>
+  <si>
+    <t>dsfsd232&amp;^</t>
+  </si>
+  <si>
+    <t>zidan@icloud.com</t>
+  </si>
+  <si>
+    <t>fdgda4567</t>
+  </si>
+  <si>
+    <t>yahyaq91@gail.com</t>
+  </si>
+  <si>
+    <t>yahyaq91yahoo.com</t>
+  </si>
+  <si>
+    <t>yahyaq91@licom</t>
+  </si>
+  <si>
+    <t>nufcotmailcom</t>
+  </si>
+  <si>
+    <t>realmadrid@liveom</t>
+  </si>
+  <si>
+    <t>cronaldo7@me.c</t>
+  </si>
+  <si>
+    <t>ronaldo9loud.com</t>
+  </si>
+  <si>
+    <t>haalandgmailcom</t>
+  </si>
+  <si>
+    <t>football@yahoocm</t>
+  </si>
+  <si>
+    <t>zidanicloud.com</t>
+  </si>
+  <si>
+    <t>football@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -476,19 +494,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DD4A45-1385-4380-889D-88CF15B37225}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.26953125" customWidth="1"/>
+    <col min="2" max="2" width="40.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,76 +514,84 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>213243314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>324112345</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -576,9 +602,10 @@
     <hyperlink ref="A5" r:id="rId4" xr:uid="{9EC1B0C7-F9FB-4606-93DA-A9CD209BFD0D}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{4F661285-4FEB-4402-A406-1DB568880342}"/>
     <hyperlink ref="A7" r:id="rId6" xr:uid="{191F02FB-407A-4B14-8804-1EC0D47C3045}"/>
-    <hyperlink ref="A8" r:id="rId7" display="kyliejenner@me.com" xr:uid="{02BA83CB-1AC0-4A35-91FB-006A15337505}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{02BA83CB-1AC0-4A35-91FB-006A15337505}"/>
     <hyperlink ref="A9" r:id="rId8" xr:uid="{C2A6C00B-EA9C-477A-9476-3C8D04C0C6B2}"/>
     <hyperlink ref="A10" r:id="rId9" xr:uid="{56A00F96-870C-4DA0-BEE0-0F42F13420AD}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{7D4890E2-84BF-4EE2-B342-74C7A4B6223B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -586,19 +613,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620C28E2-708E-44BB-B761-63885062F8E9}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -606,62 +633,98 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2">
+        <v>213243314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{6420A4C6-6966-4885-976A-8A8B12362C27}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{CF5BB034-17B1-4926-9F91-D9B85FA6E1FF}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{4E83BCDC-59F7-453B-9B84-7F78A00A3119}"/>
-    <hyperlink ref="A5" r:id="rId4" display="kyliejenner@me.com" xr:uid="{EF3BB98E-239C-43CC-A551-94CE9FCD4C1D}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{BAEC17F0-BFA5-4135-BAA4-0F2B06F84C76}"/>
-    <hyperlink ref="A7" r:id="rId6" xr:uid="{2145D067-C28B-4B9C-B346-BF64716EE0C8}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{92B7B0FB-D457-456C-ACDB-DC76DE776564}"/>
+    <hyperlink ref="A3" r:id="rId2" display="yahyaq91@yahoo.com" xr:uid="{53438704-8BC2-47AF-A53A-CE5DB3F5B0AA}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{B3883200-7D7A-4A2F-9B24-EC62EBEF29CB}"/>
+    <hyperlink ref="A5" r:id="rId4" display="nufc@hotmailcom" xr:uid="{00BE9E9C-7BB7-47DA-A965-3AB5A3BB6475}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{74FF4B21-957A-40EC-B173-DDC4CD9D5C7B}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{63C610E3-CAB2-42C5-BAE4-FD85E7F0E4C9}"/>
+    <hyperlink ref="A8" r:id="rId7" display="ronaldo9@icloud.com" xr:uid="{FF2987A4-8F22-4040-913F-F6BD026F9CEF}"/>
+    <hyperlink ref="A9" r:id="rId8" display="haaland@gmail.com" xr:uid="{145FE9AD-498C-4281-BA02-3DEE29E58F3F}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{92E1769B-12CD-49DA-B10C-B58A73A371D1}"/>
+    <hyperlink ref="A11" r:id="rId10" display="zidan@icloud.com" xr:uid="{C799B680-94CB-49D1-AA16-2FD10B7C28ED}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>